<commit_message>
add type, and env-data
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>type</t>
   </si>
@@ -22,23 +22,52 @@
     <t>value</t>
   </si>
   <si>
-    <t>date</t>
+    <t>source</t>
   </si>
   <si>
-    <t>tempreture</t>
+    <t>description</t>
   </si>
   <si>
-    <t>2023-12-10</t>
+    <t>collected_date_time</t>
   </si>
   <si>
-    <t/>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>town</t>
+  </si>
+  <si>
+    <t>wind speed</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Jenin</t>
+  </si>
+  <si>
+    <t>Jaba</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,7 +90,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,16 +104,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFd9d9d9"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -108,61 +132,94 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,15 +524,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -488,541 +550,1043 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
-        <v>45</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6">
         <v>4</v>
       </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="8">
+        <v>44907.508472222224</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44907</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="4"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="4"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="4"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="4"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="4"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="4"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="4"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="5"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="4"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="4"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="5"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="4"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="4"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="5"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="4"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="5"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="4"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="5"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="4"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="5"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="4"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="5"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="4"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="4"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="5"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="4"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="4"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="5"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="4"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="5"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="4"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="4"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="5"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="4"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="5"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="4"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="5"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="4"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="5"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="4"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="5"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="4"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="5"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="4"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="5"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="4"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="5"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="4"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="5"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="4"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="5"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="4"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="5"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="4"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="5"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="4"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="5"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="4"/>
+      <c r="A58" s="9"/>
       <c r="B58" s="9"/>
-      <c r="C58" s="5"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="10"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="12"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="10"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="10"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="10"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="10"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="10"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="12"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="10"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="10"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="10"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="10"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="10"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="12"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="10"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="12"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="10"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="12"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="10"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="12"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="10"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="12"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="10"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="12"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="10"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="10"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="12"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="10"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="10"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="10"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="10"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="10"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="12"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="10"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="12"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="10"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="12"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="10"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="12"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="10"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="10"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="10"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="12"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="10"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="12"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="10"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="12"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="10"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="12"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="10"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="12"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="10"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="12"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="10"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="12"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="10"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="12"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="10"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="12"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="10"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="12"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="10"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="12"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="10"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="12"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>